<commit_message>
column Neutral now defaults to 1 and is exclusive with other 2
</commit_message>
<xml_diff>
--- a/xlsx/myhands.xlsx
+++ b/xlsx/myhands.xlsx
@@ -1198,6 +1198,10 @@
       <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="F2">
+        <f>IF(AND(ISBLANK(D2), ISBLANK(E2)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -1209,6 +1213,10 @@
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="F3">
+        <f>IF(AND(ISBLANK(D3), ISBLANK(E3)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
@@ -1220,6 +1228,10 @@
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="F4">
+        <f>IF(AND(ISBLANK(D4), ISBLANK(E4)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
@@ -1231,6 +1243,10 @@
       <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="F5">
+        <f>IF(AND(ISBLANK(D5), ISBLANK(E5)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
@@ -1242,6 +1258,10 @@
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="F6">
+        <f>IF(AND(ISBLANK(D6), ISBLANK(E6)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
@@ -1253,6 +1273,10 @@
       <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="F7">
+        <f>IF(AND(ISBLANK(D7), ISBLANK(E7)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
@@ -1264,6 +1288,10 @@
       <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="F8">
+        <f>IF(AND(ISBLANK(D8), ISBLANK(E8)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -1275,6 +1303,10 @@
       <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="F9">
+        <f>IF(AND(ISBLANK(D9), ISBLANK(E9)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
@@ -1286,6 +1318,10 @@
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="F10">
+        <f>IF(AND(ISBLANK(D10), ISBLANK(E10)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
@@ -1297,6 +1333,10 @@
       <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="F11">
+        <f>IF(AND(ISBLANK(D11), ISBLANK(E11)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
@@ -1308,6 +1348,10 @@
       <c r="C12" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="F12">
+        <f>IF(AND(ISBLANK(D12), ISBLANK(E12)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
@@ -1319,6 +1363,10 @@
       <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="F13">
+        <f>IF(AND(ISBLANK(D13), ISBLANK(E13)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
@@ -1330,6 +1378,10 @@
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="F14">
+        <f>IF(AND(ISBLANK(D14), ISBLANK(E14)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
@@ -1341,6 +1393,10 @@
       <c r="C15" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="F15">
+        <f>IF(AND(ISBLANK(D15), ISBLANK(E15)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
@@ -1352,8 +1408,12 @@
       <c r="C16" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="F16">
+        <f>IF(AND(ISBLANK(D16), ISBLANK(E16)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1363,8 +1423,12 @@
       <c r="C17" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="F17">
+        <f>IF(AND(ISBLANK(D17), ISBLANK(E17)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1374,8 +1438,12 @@
       <c r="C18" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="F18">
+        <f>IF(AND(ISBLANK(D18), ISBLANK(E18)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1385,8 +1453,12 @@
       <c r="C19" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="F19">
+        <f>IF(AND(ISBLANK(D19), ISBLANK(E19)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1396,8 +1468,12 @@
       <c r="C20" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="F20">
+        <f>IF(AND(ISBLANK(D20), ISBLANK(E20)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1407,8 +1483,12 @@
       <c r="C21" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="F21">
+        <f>IF(AND(ISBLANK(D21), ISBLANK(E21)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1418,8 +1498,12 @@
       <c r="C22" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="F22">
+        <f>IF(AND(ISBLANK(D22), ISBLANK(E22)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1429,8 +1513,12 @@
       <c r="C23" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="F23">
+        <f>IF(AND(ISBLANK(D23), ISBLANK(E23)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1440,8 +1528,12 @@
       <c r="C24" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="F24">
+        <f>IF(AND(ISBLANK(D24), ISBLANK(E24)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1451,8 +1543,12 @@
       <c r="C25" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="F25">
+        <f>IF(AND(ISBLANK(D25), ISBLANK(E25)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1462,8 +1558,12 @@
       <c r="C26" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="F26">
+        <f>IF(AND(ISBLANK(D26), ISBLANK(E26)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1473,8 +1573,12 @@
       <c r="C27" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="F27">
+        <f>IF(AND(ISBLANK(D27), ISBLANK(E27)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1484,8 +1588,12 @@
       <c r="C28" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="F28">
+        <f>IF(AND(ISBLANK(D28), ISBLANK(E28)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1495,8 +1603,12 @@
       <c r="C29" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="F29">
+        <f>IF(AND(ISBLANK(D29), ISBLANK(E29)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1506,8 +1618,12 @@
       <c r="C30" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="F30">
+        <f>IF(AND(ISBLANK(D30), ISBLANK(E30)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1517,8 +1633,12 @@
       <c r="C31" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="F31">
+        <f>IF(AND(ISBLANK(D31), ISBLANK(E31)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -1528,8 +1648,12 @@
       <c r="C32" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="F32">
+        <f>IF(AND(ISBLANK(D32), ISBLANK(E32)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1539,8 +1663,12 @@
       <c r="C33" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="F33">
+        <f>IF(AND(ISBLANK(D33), ISBLANK(E33)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1550,8 +1678,12 @@
       <c r="C34" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="F34">
+        <f>IF(AND(ISBLANK(D34), ISBLANK(E34)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1561,8 +1693,12 @@
       <c r="C35" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="F35">
+        <f>IF(AND(ISBLANK(D35), ISBLANK(E35)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1572,8 +1708,12 @@
       <c r="C36" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="F36">
+        <f>IF(AND(ISBLANK(D36), ISBLANK(E36)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1583,8 +1723,12 @@
       <c r="C37" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="F37">
+        <f>IF(AND(ISBLANK(D37), ISBLANK(E37)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1594,8 +1738,12 @@
       <c r="C38" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="F38">
+        <f>IF(AND(ISBLANK(D38), ISBLANK(E38)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1605,8 +1753,12 @@
       <c r="C39" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="F39">
+        <f>IF(AND(ISBLANK(D39), ISBLANK(E39)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1616,8 +1768,12 @@
       <c r="C40" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="F40">
+        <f>IF(AND(ISBLANK(D40), ISBLANK(E40)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1627,8 +1783,12 @@
       <c r="C41" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="F41">
+        <f>IF(AND(ISBLANK(D41), ISBLANK(E41)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -1638,8 +1798,12 @@
       <c r="C42" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="F42">
+        <f>IF(AND(ISBLANK(D42), ISBLANK(E42)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>39</v>
       </c>
@@ -1649,8 +1813,12 @@
       <c r="C43" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="F43">
+        <f>IF(AND(ISBLANK(D43), ISBLANK(E43)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>39</v>
       </c>
@@ -1660,8 +1828,12 @@
       <c r="C44" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="F44">
+        <f>IF(AND(ISBLANK(D44), ISBLANK(E44)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -1671,8 +1843,12 @@
       <c r="C45" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="F45">
+        <f>IF(AND(ISBLANK(D45), ISBLANK(E45)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -1682,8 +1858,12 @@
       <c r="C46" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="F46">
+        <f>IF(AND(ISBLANK(D46), ISBLANK(E46)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -1693,8 +1873,12 @@
       <c r="C47" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="F47">
+        <f>IF(AND(ISBLANK(D47), ISBLANK(E47)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>39</v>
       </c>
@@ -1704,8 +1888,12 @@
       <c r="C48" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="F48">
+        <f>IF(AND(ISBLANK(D48), ISBLANK(E48)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>39</v>
       </c>
@@ -1715,8 +1903,12 @@
       <c r="C49" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="F49">
+        <f>IF(AND(ISBLANK(D49), ISBLANK(E49)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>39</v>
       </c>
@@ -1726,8 +1918,12 @@
       <c r="C50" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="F50">
+        <f>IF(AND(ISBLANK(D50), ISBLANK(E50)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>39</v>
       </c>
@@ -1737,8 +1933,12 @@
       <c r="C51" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="F51">
+        <f>IF(AND(ISBLANK(D51), ISBLANK(E51)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -1748,8 +1948,12 @@
       <c r="C52" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="F52">
+        <f>IF(AND(ISBLANK(D52), ISBLANK(E52)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>39</v>
       </c>
@@ -1759,8 +1963,12 @@
       <c r="C53" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="F53">
+        <f>IF(AND(ISBLANK(D53), ISBLANK(E53)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>39</v>
       </c>
@@ -1770,8 +1978,12 @@
       <c r="C54" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="F54">
+        <f>IF(AND(ISBLANK(D54), ISBLANK(E54)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>39</v>
       </c>
@@ -1781,8 +1993,12 @@
       <c r="C55" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="F55">
+        <f>IF(AND(ISBLANK(D55), ISBLANK(E55)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>39</v>
       </c>
@@ -1792,8 +2008,12 @@
       <c r="C56" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="F56">
+        <f>IF(AND(ISBLANK(D56), ISBLANK(E56)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>39</v>
       </c>
@@ -1803,8 +2023,12 @@
       <c r="C57" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="F57">
+        <f>IF(AND(ISBLANK(D57), ISBLANK(E57)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -1814,8 +2038,12 @@
       <c r="C58" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="F58">
+        <f>IF(AND(ISBLANK(D58), ISBLANK(E58)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -1825,8 +2053,12 @@
       <c r="C59" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="F59">
+        <f>IF(AND(ISBLANK(D59), ISBLANK(E59)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>70</v>
       </c>
@@ -1836,8 +2068,12 @@
       <c r="C60" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
+      <c r="F60">
+        <f>IF(AND(ISBLANK(D60), ISBLANK(E60)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -1847,8 +2083,12 @@
       <c r="C61" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
+      <c r="F61">
+        <f>IF(AND(ISBLANK(D61), ISBLANK(E61)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -1858,8 +2098,12 @@
       <c r="C62" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="F62">
+        <f>IF(AND(ISBLANK(D62), ISBLANK(E62)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -1869,8 +2113,12 @@
       <c r="C63" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
+      <c r="F63">
+        <f>IF(AND(ISBLANK(D63), ISBLANK(E63)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -1880,8 +2128,12 @@
       <c r="C64" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="F64">
+        <f>IF(AND(ISBLANK(D64), ISBLANK(E64)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -1891,8 +2143,12 @@
       <c r="C65" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="F65">
+        <f>IF(AND(ISBLANK(D65), ISBLANK(E65)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -1902,8 +2158,12 @@
       <c r="C66" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
+      <c r="F66">
+        <f>IF(AND(ISBLANK(D66), ISBLANK(E66)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -1913,8 +2173,12 @@
       <c r="C67" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="F67">
+        <f>IF(AND(ISBLANK(D67), ISBLANK(E67)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -1924,8 +2188,12 @@
       <c r="C68" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="F68">
+        <f>IF(AND(ISBLANK(D68), ISBLANK(E68)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -1935,8 +2203,12 @@
       <c r="C69" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="F69">
+        <f>IF(AND(ISBLANK(D69), ISBLANK(E69)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -1946,8 +2218,12 @@
       <c r="C70" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
+      <c r="F70">
+        <f>IF(AND(ISBLANK(D70), ISBLANK(E70)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -1957,8 +2233,12 @@
       <c r="C71" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="F71">
+        <f>IF(AND(ISBLANK(D71), ISBLANK(E71)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -1968,8 +2248,12 @@
       <c r="C72" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
+      <c r="F72">
+        <f>IF(AND(ISBLANK(D72), ISBLANK(E72)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -1979,8 +2263,12 @@
       <c r="C73" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="F73">
+        <f>IF(AND(ISBLANK(D73), ISBLANK(E73)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>70</v>
       </c>
@@ -1990,8 +2278,12 @@
       <c r="C74" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
+      <c r="F74">
+        <f>IF(AND(ISBLANK(D74), ISBLANK(E74)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>70</v>
       </c>
@@ -2001,8 +2293,12 @@
       <c r="C75" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="F75">
+        <f>IF(AND(ISBLANK(D75), ISBLANK(E75)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>70</v>
       </c>
@@ -2012,8 +2308,12 @@
       <c r="C76" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="F76">
+        <f>IF(AND(ISBLANK(D76), ISBLANK(E76)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>70</v>
       </c>
@@ -2023,8 +2323,12 @@
       <c r="C77" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
+      <c r="F77">
+        <f>IF(AND(ISBLANK(D77), ISBLANK(E77)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>70</v>
       </c>
@@ -2034,8 +2338,12 @@
       <c r="C78" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="79" spans="1:3">
+      <c r="F78">
+        <f>IF(AND(ISBLANK(D78), ISBLANK(E78)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>70</v>
       </c>
@@ -2045,8 +2353,12 @@
       <c r="C79" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="F79">
+        <f>IF(AND(ISBLANK(D79), ISBLANK(E79)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>70</v>
       </c>
@@ -2056,8 +2368,12 @@
       <c r="C80" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="81" spans="1:3">
+      <c r="F80">
+        <f>IF(AND(ISBLANK(D80), ISBLANK(E80)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>70</v>
       </c>
@@ -2067,8 +2383,12 @@
       <c r="C81" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="82" spans="1:3">
+      <c r="F81">
+        <f>IF(AND(ISBLANK(D81), ISBLANK(E81)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>70</v>
       </c>
@@ -2078,8 +2398,12 @@
       <c r="C82" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
+      <c r="F82">
+        <f>IF(AND(ISBLANK(D82), ISBLANK(E82)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
       <c r="A83" t="s">
         <v>70</v>
       </c>
@@ -2089,8 +2413,12 @@
       <c r="C83" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="84" spans="1:3">
+      <c r="F83">
+        <f>IF(AND(ISBLANK(D83), ISBLANK(E83)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
         <v>70</v>
       </c>
@@ -2100,8 +2428,12 @@
       <c r="C84" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="85" spans="1:3">
+      <c r="F84">
+        <f>IF(AND(ISBLANK(D84), ISBLANK(E84)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
         <v>70</v>
       </c>
@@ -2111,8 +2443,12 @@
       <c r="C85" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="86" spans="1:3">
+      <c r="F85">
+        <f>IF(AND(ISBLANK(D85), ISBLANK(E85)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
         <v>101</v>
       </c>
@@ -2122,8 +2458,12 @@
       <c r="C86" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="87" spans="1:3">
+      <c r="F86">
+        <f>IF(AND(ISBLANK(D86), ISBLANK(E86)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
       <c r="A87" t="s">
         <v>101</v>
       </c>
@@ -2133,8 +2473,12 @@
       <c r="C87" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="F87">
+        <f>IF(AND(ISBLANK(D87), ISBLANK(E87)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88" t="s">
         <v>101</v>
       </c>
@@ -2144,8 +2488,12 @@
       <c r="C88" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
+      <c r="F88">
+        <f>IF(AND(ISBLANK(D88), ISBLANK(E88)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
         <v>101</v>
       </c>
@@ -2155,8 +2503,12 @@
       <c r="C89" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="90" spans="1:3">
+      <c r="F89">
+        <f>IF(AND(ISBLANK(D89), ISBLANK(E89)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
         <v>101</v>
       </c>
@@ -2166,8 +2518,12 @@
       <c r="C90" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="91" spans="1:3">
+      <c r="F90">
+        <f>IF(AND(ISBLANK(D90), ISBLANK(E90)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
         <v>101</v>
       </c>
@@ -2177,8 +2533,12 @@
       <c r="C91" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="92" spans="1:3">
+      <c r="F91">
+        <f>IF(AND(ISBLANK(D91), ISBLANK(E91)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
         <v>101</v>
       </c>
@@ -2188,8 +2548,12 @@
       <c r="C92" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="93" spans="1:3">
+      <c r="F92">
+        <f>IF(AND(ISBLANK(D92), ISBLANK(E92)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
       <c r="A93" t="s">
         <v>101</v>
       </c>
@@ -2199,8 +2563,12 @@
       <c r="C93" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
+      <c r="F93">
+        <f>IF(AND(ISBLANK(D93), ISBLANK(E93)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
         <v>101</v>
       </c>
@@ -2210,8 +2578,12 @@
       <c r="C94" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="95" spans="1:3">
+      <c r="F94">
+        <f>IF(AND(ISBLANK(D94), ISBLANK(E94)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>101</v>
       </c>
@@ -2221,8 +2593,12 @@
       <c r="C95" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="96" spans="1:3">
+      <c r="F95">
+        <f>IF(AND(ISBLANK(D95), ISBLANK(E95)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
         <v>101</v>
       </c>
@@ -2232,8 +2608,12 @@
       <c r="C96" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="97" spans="1:3">
+      <c r="F96">
+        <f>IF(AND(ISBLANK(D96), ISBLANK(E96)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
         <v>101</v>
       </c>
@@ -2243,8 +2623,12 @@
       <c r="C97" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="98" spans="1:3">
+      <c r="F97">
+        <f>IF(AND(ISBLANK(D97), ISBLANK(E97)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
       <c r="A98" t="s">
         <v>101</v>
       </c>
@@ -2254,8 +2638,12 @@
       <c r="C98" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="99" spans="1:3">
+      <c r="F98">
+        <f>IF(AND(ISBLANK(D98), ISBLANK(E98)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
       <c r="A99" t="s">
         <v>101</v>
       </c>
@@ -2265,8 +2653,12 @@
       <c r="C99" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="100" spans="1:3">
+      <c r="F99">
+        <f>IF(AND(ISBLANK(D99), ISBLANK(E99)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
       <c r="A100" t="s">
         <v>101</v>
       </c>
@@ -2276,8 +2668,12 @@
       <c r="C100" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="101" spans="1:3">
+      <c r="F100">
+        <f>IF(AND(ISBLANK(D100), ISBLANK(E100)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
       <c r="A101" t="s">
         <v>101</v>
       </c>
@@ -2287,8 +2683,12 @@
       <c r="C101" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="102" spans="1:3">
+      <c r="F101">
+        <f>IF(AND(ISBLANK(D101), ISBLANK(E101)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -2298,8 +2698,12 @@
       <c r="C102" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="103" spans="1:3">
+      <c r="F102">
+        <f>IF(AND(ISBLANK(D102), ISBLANK(E102)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -2309,8 +2713,12 @@
       <c r="C103" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="104" spans="1:3">
+      <c r="F103">
+        <f>IF(AND(ISBLANK(D103), ISBLANK(E103)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
       <c r="A104" t="s">
         <v>101</v>
       </c>
@@ -2320,8 +2728,12 @@
       <c r="C104" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="105" spans="1:3">
+      <c r="F104">
+        <f>IF(AND(ISBLANK(D104), ISBLANK(E104)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
       <c r="A105" t="s">
         <v>101</v>
       </c>
@@ -2331,8 +2743,12 @@
       <c r="C105" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="106" spans="1:3">
+      <c r="F105">
+        <f>IF(AND(ISBLANK(D105), ISBLANK(E105)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
       <c r="A106" t="s">
         <v>101</v>
       </c>
@@ -2342,8 +2758,12 @@
       <c r="C106" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="107" spans="1:3">
+      <c r="F106">
+        <f>IF(AND(ISBLANK(D106), ISBLANK(E106)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
       <c r="A107" t="s">
         <v>101</v>
       </c>
@@ -2353,8 +2773,12 @@
       <c r="C107" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="108" spans="1:3">
+      <c r="F107">
+        <f>IF(AND(ISBLANK(D107), ISBLANK(E107)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
       <c r="A108" t="s">
         <v>101</v>
       </c>
@@ -2364,8 +2788,12 @@
       <c r="C108" s="2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="109" spans="1:3">
+      <c r="F108">
+        <f>IF(AND(ISBLANK(D108), ISBLANK(E108)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
       <c r="A109" t="s">
         <v>101</v>
       </c>
@@ -2375,8 +2803,12 @@
       <c r="C109" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="110" spans="1:3">
+      <c r="F109">
+        <f>IF(AND(ISBLANK(D109), ISBLANK(E109)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
       <c r="A110" t="s">
         <v>101</v>
       </c>
@@ -2386,8 +2818,12 @@
       <c r="C110" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="111" spans="1:3">
+      <c r="F110">
+        <f>IF(AND(ISBLANK(D110), ISBLANK(E110)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
       <c r="A111" t="s">
         <v>101</v>
       </c>
@@ -2397,8 +2833,12 @@
       <c r="C111" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="112" spans="1:3">
+      <c r="F111">
+        <f>IF(AND(ISBLANK(D111), ISBLANK(E111)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
       <c r="A112" t="s">
         <v>101</v>
       </c>
@@ -2408,8 +2848,12 @@
       <c r="C112" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="113" spans="1:3">
+      <c r="F112">
+        <f>IF(AND(ISBLANK(D112), ISBLANK(E112)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
       <c r="A113" t="s">
         <v>101</v>
       </c>
@@ -2419,8 +2863,12 @@
       <c r="C113" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="114" spans="1:3">
+      <c r="F113">
+        <f>IF(AND(ISBLANK(D113), ISBLANK(E113)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
       <c r="A114" t="s">
         <v>101</v>
       </c>
@@ -2430,8 +2878,12 @@
       <c r="C114" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="115" spans="1:3">
+      <c r="F114">
+        <f>IF(AND(ISBLANK(D114), ISBLANK(E114)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
       <c r="A115" t="s">
         <v>101</v>
       </c>
@@ -2441,8 +2893,12 @@
       <c r="C115" s="2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="116" spans="1:3">
+      <c r="F115">
+        <f>IF(AND(ISBLANK(D115), ISBLANK(E115)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
       <c r="A116" t="s">
         <v>101</v>
       </c>
@@ -2452,8 +2908,12 @@
       <c r="C116" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="117" spans="1:3">
+      <c r="F116">
+        <f>IF(AND(ISBLANK(D116), ISBLANK(E116)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
       <c r="A117" t="s">
         <v>101</v>
       </c>
@@ -2463,8 +2923,12 @@
       <c r="C117" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="118" spans="1:3">
+      <c r="F117">
+        <f>IF(AND(ISBLANK(D117), ISBLANK(E117)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
       <c r="A118" t="s">
         <v>101</v>
       </c>
@@ -2474,8 +2938,12 @@
       <c r="C118" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="119" spans="1:3">
+      <c r="F118">
+        <f>IF(AND(ISBLANK(D118), ISBLANK(E118)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
       <c r="A119" t="s">
         <v>101</v>
       </c>
@@ -2485,8 +2953,12 @@
       <c r="C119" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="120" spans="1:3">
+      <c r="F119">
+        <f>IF(AND(ISBLANK(D119), ISBLANK(E119)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
       <c r="A120" t="s">
         <v>101</v>
       </c>
@@ -2496,8 +2968,12 @@
       <c r="C120" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="121" spans="1:3">
+      <c r="F120">
+        <f>IF(AND(ISBLANK(D120), ISBLANK(E120)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
       <c r="A121" t="s">
         <v>101</v>
       </c>
@@ -2507,8 +2983,12 @@
       <c r="C121" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="122" spans="1:3">
+      <c r="F121">
+        <f>IF(AND(ISBLANK(D121), ISBLANK(E121)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
       <c r="A122" t="s">
         <v>101</v>
       </c>
@@ -2518,8 +2998,12 @@
       <c r="C122" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="123" spans="1:3">
+      <c r="F122">
+        <f>IF(AND(ISBLANK(D122), ISBLANK(E122)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
       <c r="A123" t="s">
         <v>101</v>
       </c>
@@ -2529,8 +3013,12 @@
       <c r="C123" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="124" spans="1:3">
+      <c r="F123">
+        <f>IF(AND(ISBLANK(D123), ISBLANK(E123)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
       <c r="A124" t="s">
         <v>101</v>
       </c>
@@ -2540,8 +3028,12 @@
       <c r="C124" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="125" spans="1:3">
+      <c r="F124">
+        <f>IF(AND(ISBLANK(D124), ISBLANK(E124)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
       <c r="A125" t="s">
         <v>101</v>
       </c>
@@ -2551,8 +3043,12 @@
       <c r="C125" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="126" spans="1:3">
+      <c r="F125">
+        <f>IF(AND(ISBLANK(D125), ISBLANK(E125)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
       <c r="A126" t="s">
         <v>101</v>
       </c>
@@ -2562,8 +3058,12 @@
       <c r="C126" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="127" spans="1:3">
+      <c r="F126">
+        <f>IF(AND(ISBLANK(D126), ISBLANK(E126)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
       <c r="A127" t="s">
         <v>101</v>
       </c>
@@ -2573,8 +3073,12 @@
       <c r="C127" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="128" spans="1:3">
+      <c r="F127">
+        <f>IF(AND(ISBLANK(D127), ISBLANK(E127)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
       <c r="A128" t="s">
         <v>101</v>
       </c>
@@ -2584,8 +3088,12 @@
       <c r="C128" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="129" spans="1:3">
+      <c r="F128">
+        <f>IF(AND(ISBLANK(D128), ISBLANK(E128)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
       <c r="A129" t="s">
         <v>101</v>
       </c>
@@ -2595,8 +3103,12 @@
       <c r="C129" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="130" spans="1:3">
+      <c r="F129">
+        <f>IF(AND(ISBLANK(D129), ISBLANK(E129)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
       <c r="A130" t="s">
         <v>101</v>
       </c>
@@ -2606,8 +3118,12 @@
       <c r="C130" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="131" spans="1:3">
+      <c r="F130">
+        <f>IF(AND(ISBLANK(D130), ISBLANK(E130)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
       <c r="A131" t="s">
         <v>101</v>
       </c>
@@ -2617,8 +3133,12 @@
       <c r="C131" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="132" spans="1:3">
+      <c r="F131">
+        <f>IF(AND(ISBLANK(D131), ISBLANK(E131)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
       <c r="A132" t="s">
         <v>101</v>
       </c>
@@ -2628,8 +3148,12 @@
       <c r="C132" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="133" spans="1:3">
+      <c r="F132">
+        <f>IF(AND(ISBLANK(D132), ISBLANK(E132)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
       <c r="A133" t="s">
         <v>101</v>
       </c>
@@ -2639,8 +3163,12 @@
       <c r="C133" s="2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="134" spans="1:3">
+      <c r="F133">
+        <f>IF(AND(ISBLANK(D133), ISBLANK(E133)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
       <c r="A134" t="s">
         <v>153</v>
       </c>
@@ -2650,8 +3178,12 @@
       <c r="C134" s="2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="135" spans="1:3">
+      <c r="F134">
+        <f>IF(AND(ISBLANK(D134), ISBLANK(E134)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
       <c r="A135" t="s">
         <v>153</v>
       </c>
@@ -2661,8 +3193,12 @@
       <c r="C135" s="2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="136" spans="1:3">
+      <c r="F135">
+        <f>IF(AND(ISBLANK(D135), ISBLANK(E135)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
       <c r="A136" t="s">
         <v>153</v>
       </c>
@@ -2672,8 +3208,12 @@
       <c r="C136" s="2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="137" spans="1:3">
+      <c r="F136">
+        <f>IF(AND(ISBLANK(D136), ISBLANK(E136)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
       <c r="A137" t="s">
         <v>153</v>
       </c>
@@ -2683,8 +3223,12 @@
       <c r="C137" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="138" spans="1:3">
+      <c r="F137">
+        <f>IF(AND(ISBLANK(D137), ISBLANK(E137)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
       <c r="A138" t="s">
         <v>153</v>
       </c>
@@ -2694,8 +3238,12 @@
       <c r="C138" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="139" spans="1:3">
+      <c r="F138">
+        <f>IF(AND(ISBLANK(D138), ISBLANK(E138)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
       <c r="A139" t="s">
         <v>153</v>
       </c>
@@ -2705,8 +3253,12 @@
       <c r="C139" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="140" spans="1:3">
+      <c r="F139">
+        <f>IF(AND(ISBLANK(D139), ISBLANK(E139)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
       <c r="A140" t="s">
         <v>153</v>
       </c>
@@ -2716,8 +3268,12 @@
       <c r="C140" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="141" spans="1:3">
+      <c r="F140">
+        <f>IF(AND(ISBLANK(D140), ISBLANK(E140)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
       <c r="A141" t="s">
         <v>153</v>
       </c>
@@ -2727,8 +3283,12 @@
       <c r="C141" s="2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="142" spans="1:3">
+      <c r="F141">
+        <f>IF(AND(ISBLANK(D141), ISBLANK(E141)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
       <c r="A142" t="s">
         <v>153</v>
       </c>
@@ -2738,8 +3298,12 @@
       <c r="C142" s="2" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="143" spans="1:3">
+      <c r="F142">
+        <f>IF(AND(ISBLANK(D142), ISBLANK(E142)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
       <c r="A143" t="s">
         <v>153</v>
       </c>
@@ -2749,8 +3313,12 @@
       <c r="C143" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="144" spans="1:3">
+      <c r="F143">
+        <f>IF(AND(ISBLANK(D143), ISBLANK(E143)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
       <c r="A144" t="s">
         <v>153</v>
       </c>
@@ -2760,8 +3328,12 @@
       <c r="C144" s="2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="145" spans="1:3">
+      <c r="F144">
+        <f>IF(AND(ISBLANK(D144), ISBLANK(E144)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
       <c r="A145" t="s">
         <v>153</v>
       </c>
@@ -2771,8 +3343,12 @@
       <c r="C145" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="146" spans="1:3">
+      <c r="F145">
+        <f>IF(AND(ISBLANK(D145), ISBLANK(E145)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
       <c r="A146" t="s">
         <v>153</v>
       </c>
@@ -2782,8 +3358,12 @@
       <c r="C146" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="147" spans="1:3">
+      <c r="F146">
+        <f>IF(AND(ISBLANK(D146), ISBLANK(E146)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
       <c r="A147" t="s">
         <v>153</v>
       </c>
@@ -2793,8 +3373,12 @@
       <c r="C147" s="2" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="148" spans="1:3">
+      <c r="F147">
+        <f>IF(AND(ISBLANK(D147), ISBLANK(E147)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
       <c r="A148" t="s">
         <v>153</v>
       </c>
@@ -2804,8 +3388,12 @@
       <c r="C148" s="2" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="149" spans="1:3">
+      <c r="F148">
+        <f>IF(AND(ISBLANK(D148), ISBLANK(E148)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
       <c r="A149" t="s">
         <v>153</v>
       </c>
@@ -2815,8 +3403,12 @@
       <c r="C149" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="150" spans="1:3">
+      <c r="F149">
+        <f>IF(AND(ISBLANK(D149), ISBLANK(E149)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
       <c r="A150" t="s">
         <v>153</v>
       </c>
@@ -2826,8 +3418,12 @@
       <c r="C150" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="151" spans="1:3">
+      <c r="F150">
+        <f>IF(AND(ISBLANK(D150), ISBLANK(E150)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
       <c r="A151" t="s">
         <v>153</v>
       </c>
@@ -2837,8 +3433,12 @@
       <c r="C151" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="152" spans="1:3">
+      <c r="F151">
+        <f>IF(AND(ISBLANK(D151), ISBLANK(E151)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
       <c r="A152" t="s">
         <v>153</v>
       </c>
@@ -2848,8 +3448,12 @@
       <c r="C152" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="153" spans="1:3">
+      <c r="F152">
+        <f>IF(AND(ISBLANK(D152), ISBLANK(E152)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
       <c r="A153" t="s">
         <v>153</v>
       </c>
@@ -2859,8 +3463,12 @@
       <c r="C153" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="154" spans="1:3">
+      <c r="F153">
+        <f>IF(AND(ISBLANK(D153), ISBLANK(E153)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -2870,8 +3478,12 @@
       <c r="C154" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="155" spans="1:3">
+      <c r="F154">
+        <f>IF(AND(ISBLANK(D154), ISBLANK(E154)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
       <c r="A155" t="s">
         <v>153</v>
       </c>
@@ -2881,8 +3493,12 @@
       <c r="C155" s="2" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="156" spans="1:3">
+      <c r="F155">
+        <f>IF(AND(ISBLANK(D155), ISBLANK(E155)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
       <c r="A156" t="s">
         <v>153</v>
       </c>
@@ -2892,8 +3508,12 @@
       <c r="C156" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="157" spans="1:3">
+      <c r="F156">
+        <f>IF(AND(ISBLANK(D156), ISBLANK(E156)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
       <c r="A157" t="s">
         <v>153</v>
       </c>
@@ -2903,8 +3523,12 @@
       <c r="C157" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="158" spans="1:3">
+      <c r="F157">
+        <f>IF(AND(ISBLANK(D157), ISBLANK(E157)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
       <c r="A158" t="s">
         <v>153</v>
       </c>
@@ -2914,8 +3538,12 @@
       <c r="C158" s="2" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="159" spans="1:3">
+      <c r="F158">
+        <f>IF(AND(ISBLANK(D158), ISBLANK(E158)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
       <c r="A159" t="s">
         <v>153</v>
       </c>
@@ -2925,8 +3553,12 @@
       <c r="C159" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="160" spans="1:3">
+      <c r="F159">
+        <f>IF(AND(ISBLANK(D159), ISBLANK(E159)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
       <c r="A160" t="s">
         <v>153</v>
       </c>
@@ -2936,8 +3568,12 @@
       <c r="C160" s="2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="161" spans="1:3">
+      <c r="F160">
+        <f>IF(AND(ISBLANK(D160), ISBLANK(E160)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
       <c r="A161" t="s">
         <v>153</v>
       </c>
@@ -2947,8 +3583,12 @@
       <c r="C161" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="162" spans="1:3">
+      <c r="F161">
+        <f>IF(AND(ISBLANK(D161), ISBLANK(E161)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
       <c r="A162" t="s">
         <v>153</v>
       </c>
@@ -2958,8 +3598,12 @@
       <c r="C162" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="163" spans="1:3">
+      <c r="F162">
+        <f>IF(AND(ISBLANK(D162), ISBLANK(E162)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
       <c r="A163" t="s">
         <v>153</v>
       </c>
@@ -2969,8 +3613,12 @@
       <c r="C163" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="164" spans="1:3">
+      <c r="F163">
+        <f>IF(AND(ISBLANK(D163), ISBLANK(E163)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
       <c r="A164" t="s">
         <v>153</v>
       </c>
@@ -2980,8 +3628,12 @@
       <c r="C164" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="165" spans="1:3">
+      <c r="F164">
+        <f>IF(AND(ISBLANK(D164), ISBLANK(E164)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
       <c r="A165" t="s">
         <v>153</v>
       </c>
@@ -2991,8 +3643,12 @@
       <c r="C165" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="166" spans="1:3">
+      <c r="F165">
+        <f>IF(AND(ISBLANK(D165), ISBLANK(E165)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
       <c r="A166" t="s">
         <v>153</v>
       </c>
@@ -3002,8 +3658,12 @@
       <c r="C166" s="2" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="167" spans="1:3">
+      <c r="F166">
+        <f>IF(AND(ISBLANK(D166), ISBLANK(E166)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6">
       <c r="A167" t="s">
         <v>153</v>
       </c>
@@ -3013,8 +3673,12 @@
       <c r="C167" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="168" spans="1:3">
+      <c r="F167">
+        <f>IF(AND(ISBLANK(D167), ISBLANK(E167)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
       <c r="A168" t="s">
         <v>153</v>
       </c>
@@ -3024,8 +3688,12 @@
       <c r="C168" s="2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="169" spans="1:3">
+      <c r="F168">
+        <f>IF(AND(ISBLANK(D168), ISBLANK(E168)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
       <c r="A169" t="s">
         <v>153</v>
       </c>
@@ -3035,8 +3703,12 @@
       <c r="C169" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="170" spans="1:3">
+      <c r="F169">
+        <f>IF(AND(ISBLANK(D169), ISBLANK(E169)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
       <c r="A170" t="s">
         <v>153</v>
       </c>
@@ -3046,8 +3718,12 @@
       <c r="C170" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="171" spans="1:3">
+      <c r="F170">
+        <f>IF(AND(ISBLANK(D170), ISBLANK(E170)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
       <c r="A171" t="s">
         <v>153</v>
       </c>
@@ -3057,8 +3733,12 @@
       <c r="C171" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="172" spans="1:3">
+      <c r="F171">
+        <f>IF(AND(ISBLANK(D171), ISBLANK(E171)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
       <c r="A172" t="s">
         <v>153</v>
       </c>
@@ -3068,8 +3748,12 @@
       <c r="C172" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="173" spans="1:3">
+      <c r="F172">
+        <f>IF(AND(ISBLANK(D172), ISBLANK(E172)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
       <c r="A173" t="s">
         <v>153</v>
       </c>
@@ -3079,8 +3763,12 @@
       <c r="C173" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="174" spans="1:3">
+      <c r="F173">
+        <f>IF(AND(ISBLANK(D173), ISBLANK(E173)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
       <c r="A174" t="s">
         <v>153</v>
       </c>
@@ -3090,8 +3778,12 @@
       <c r="C174" s="2" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="175" spans="1:3">
+      <c r="F174">
+        <f>IF(AND(ISBLANK(D174), ISBLANK(E174)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
       <c r="A175" t="s">
         <v>153</v>
       </c>
@@ -3101,8 +3793,12 @@
       <c r="C175" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="176" spans="1:3">
+      <c r="F175">
+        <f>IF(AND(ISBLANK(D175), ISBLANK(E175)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
       <c r="A176" t="s">
         <v>153</v>
       </c>
@@ -3112,8 +3808,12 @@
       <c r="C176" s="2" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="177" spans="1:3">
+      <c r="F176">
+        <f>IF(AND(ISBLANK(D176), ISBLANK(E176)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
       <c r="A177" t="s">
         <v>153</v>
       </c>
@@ -3123,8 +3823,12 @@
       <c r="C177" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="178" spans="1:3">
+      <c r="F177">
+        <f>IF(AND(ISBLANK(D177), ISBLANK(E177)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6">
       <c r="A178" t="s">
         <v>153</v>
       </c>
@@ -3134,8 +3838,12 @@
       <c r="C178" s="2" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="179" spans="1:3">
+      <c r="F178">
+        <f>IF(AND(ISBLANK(D178), ISBLANK(E178)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
       <c r="A179" t="s">
         <v>153</v>
       </c>
@@ -3145,8 +3853,12 @@
       <c r="C179" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="180" spans="1:3">
+      <c r="F179">
+        <f>IF(AND(ISBLANK(D179), ISBLANK(E179)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
       <c r="A180" t="s">
         <v>153</v>
       </c>
@@ -3156,8 +3868,12 @@
       <c r="C180" s="2" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="181" spans="1:3">
+      <c r="F180">
+        <f>IF(AND(ISBLANK(D180), ISBLANK(E180)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
       <c r="A181" t="s">
         <v>153</v>
       </c>
@@ -3167,8 +3883,12 @@
       <c r="C181" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="182" spans="1:3">
+      <c r="F181">
+        <f>IF(AND(ISBLANK(D181), ISBLANK(E181)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6">
       <c r="A182" t="s">
         <v>205</v>
       </c>
@@ -3178,8 +3898,12 @@
       <c r="C182" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="183" spans="1:3">
+      <c r="F182">
+        <f>IF(AND(ISBLANK(D182), ISBLANK(E182)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6">
       <c r="A183" t="s">
         <v>205</v>
       </c>
@@ -3189,8 +3913,12 @@
       <c r="C183" s="2" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="184" spans="1:3">
+      <c r="F183">
+        <f>IF(AND(ISBLANK(D183), ISBLANK(E183)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6">
       <c r="A184" t="s">
         <v>205</v>
       </c>
@@ -3200,8 +3928,12 @@
       <c r="C184" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="185" spans="1:3">
+      <c r="F184">
+        <f>IF(AND(ISBLANK(D184), ISBLANK(E184)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6">
       <c r="A185" t="s">
         <v>205</v>
       </c>
@@ -3211,8 +3943,12 @@
       <c r="C185" s="2" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="186" spans="1:3">
+      <c r="F185">
+        <f>IF(AND(ISBLANK(D185), ISBLANK(E185)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6">
       <c r="A186" t="s">
         <v>205</v>
       </c>
@@ -3222,8 +3958,12 @@
       <c r="C186" s="2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="187" spans="1:3">
+      <c r="F186">
+        <f>IF(AND(ISBLANK(D186), ISBLANK(E186)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6">
       <c r="A187" t="s">
         <v>205</v>
       </c>
@@ -3233,8 +3973,12 @@
       <c r="C187" s="2" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="188" spans="1:3">
+      <c r="F187">
+        <f>IF(AND(ISBLANK(D187), ISBLANK(E187)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6">
       <c r="A188" t="s">
         <v>205</v>
       </c>
@@ -3244,8 +3988,12 @@
       <c r="C188" s="2" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="189" spans="1:3">
+      <c r="F188">
+        <f>IF(AND(ISBLANK(D188), ISBLANK(E188)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6">
       <c r="A189" t="s">
         <v>205</v>
       </c>
@@ -3255,8 +4003,12 @@
       <c r="C189" s="2" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="190" spans="1:3">
+      <c r="F189">
+        <f>IF(AND(ISBLANK(D189), ISBLANK(E189)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6">
       <c r="A190" t="s">
         <v>205</v>
       </c>
@@ -3266,8 +4018,12 @@
       <c r="C190" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="191" spans="1:3">
+      <c r="F190">
+        <f>IF(AND(ISBLANK(D190), ISBLANK(E190)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6">
       <c r="A191" t="s">
         <v>205</v>
       </c>
@@ -3277,8 +4033,12 @@
       <c r="C191" s="2" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="192" spans="1:3">
+      <c r="F191">
+        <f>IF(AND(ISBLANK(D191), ISBLANK(E191)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6">
       <c r="A192" t="s">
         <v>205</v>
       </c>
@@ -3288,8 +4048,12 @@
       <c r="C192" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="193" spans="1:3">
+      <c r="F192">
+        <f>IF(AND(ISBLANK(D192), ISBLANK(E192)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6">
       <c r="A193" t="s">
         <v>205</v>
       </c>
@@ -3299,8 +4063,12 @@
       <c r="C193" s="2" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="194" spans="1:3">
+      <c r="F193">
+        <f>IF(AND(ISBLANK(D193), ISBLANK(E193)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6">
       <c r="A194" t="s">
         <v>205</v>
       </c>
@@ -3310,8 +4078,12 @@
       <c r="C194" s="2" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="195" spans="1:3">
+      <c r="F194">
+        <f>IF(AND(ISBLANK(D194), ISBLANK(E194)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6">
       <c r="A195" t="s">
         <v>205</v>
       </c>
@@ -3321,8 +4093,12 @@
       <c r="C195" s="2" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="196" spans="1:3">
+      <c r="F195">
+        <f>IF(AND(ISBLANK(D195), ISBLANK(E195)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6">
       <c r="A196" t="s">
         <v>205</v>
       </c>
@@ -3332,8 +4108,12 @@
       <c r="C196" s="2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="197" spans="1:3">
+      <c r="F196">
+        <f>IF(AND(ISBLANK(D196), ISBLANK(E196)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6">
       <c r="A197" t="s">
         <v>205</v>
       </c>
@@ -3343,8 +4123,12 @@
       <c r="C197" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="198" spans="1:3">
+      <c r="F197">
+        <f>IF(AND(ISBLANK(D197), ISBLANK(E197)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6">
       <c r="A198" t="s">
         <v>205</v>
       </c>
@@ -3354,8 +4138,12 @@
       <c r="C198" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="199" spans="1:3">
+      <c r="F198">
+        <f>IF(AND(ISBLANK(D198), ISBLANK(E198)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6">
       <c r="A199" t="s">
         <v>205</v>
       </c>
@@ -3365,8 +4153,12 @@
       <c r="C199" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="200" spans="1:3">
+      <c r="F199">
+        <f>IF(AND(ISBLANK(D199), ISBLANK(E199)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6">
       <c r="A200" t="s">
         <v>205</v>
       </c>
@@ -3376,8 +4168,12 @@
       <c r="C200" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="201" spans="1:3">
+      <c r="F200">
+        <f>IF(AND(ISBLANK(D200), ISBLANK(E200)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6">
       <c r="A201" t="s">
         <v>205</v>
       </c>
@@ -3387,8 +4183,12 @@
       <c r="C201" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="202" spans="1:3">
+      <c r="F201">
+        <f>IF(AND(ISBLANK(D201), ISBLANK(E201)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6">
       <c r="A202" t="s">
         <v>205</v>
       </c>
@@ -3398,8 +4198,12 @@
       <c r="C202" s="2" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="203" spans="1:3">
+      <c r="F202">
+        <f>IF(AND(ISBLANK(D202), ISBLANK(E202)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6">
       <c r="A203" t="s">
         <v>205</v>
       </c>
@@ -3409,8 +4213,12 @@
       <c r="C203" s="2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="204" spans="1:3">
+      <c r="F203">
+        <f>IF(AND(ISBLANK(D203), ISBLANK(E203)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6">
       <c r="A204" t="s">
         <v>205</v>
       </c>
@@ -3420,8 +4228,12 @@
       <c r="C204" s="2" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="205" spans="1:3">
+      <c r="F204">
+        <f>IF(AND(ISBLANK(D204), ISBLANK(E204)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6">
       <c r="A205" t="s">
         <v>205</v>
       </c>
@@ -3431,8 +4243,12 @@
       <c r="C205" s="2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="206" spans="1:3">
+      <c r="F205">
+        <f>IF(AND(ISBLANK(D205), ISBLANK(E205)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -3442,8 +4258,12 @@
       <c r="C206" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="207" spans="1:3">
+      <c r="F206">
+        <f>IF(AND(ISBLANK(D206), ISBLANK(E206)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6">
       <c r="A207" t="s">
         <v>205</v>
       </c>
@@ -3453,8 +4273,12 @@
       <c r="C207" s="2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="208" spans="1:3">
+      <c r="F207">
+        <f>IF(AND(ISBLANK(D207), ISBLANK(E207)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6">
       <c r="A208" t="s">
         <v>205</v>
       </c>
@@ -3464,8 +4288,12 @@
       <c r="C208" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="209" spans="1:3">
+      <c r="F208">
+        <f>IF(AND(ISBLANK(D208), ISBLANK(E208)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6">
       <c r="A209" t="s">
         <v>205</v>
       </c>
@@ -3475,8 +4303,12 @@
       <c r="C209" s="2" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="210" spans="1:3">
+      <c r="F209">
+        <f>IF(AND(ISBLANK(D209), ISBLANK(E209)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6">
       <c r="A210" t="s">
         <v>205</v>
       </c>
@@ -3486,8 +4318,12 @@
       <c r="C210" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="211" spans="1:3">
+      <c r="F210">
+        <f>IF(AND(ISBLANK(D210), ISBLANK(E210)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6">
       <c r="A211" t="s">
         <v>205</v>
       </c>
@@ -3497,8 +4333,12 @@
       <c r="C211" s="2" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="212" spans="1:3">
+      <c r="F211">
+        <f>IF(AND(ISBLANK(D211), ISBLANK(E211)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6">
       <c r="A212" t="s">
         <v>205</v>
       </c>
@@ -3508,8 +4348,12 @@
       <c r="C212" s="2" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="213" spans="1:3">
+      <c r="F212">
+        <f>IF(AND(ISBLANK(D212), ISBLANK(E212)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6">
       <c r="A213" t="s">
         <v>205</v>
       </c>
@@ -3519,8 +4363,12 @@
       <c r="C213" s="2" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="214" spans="1:3">
+      <c r="F213">
+        <f>IF(AND(ISBLANK(D213), ISBLANK(E213)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6">
       <c r="A214" t="s">
         <v>205</v>
       </c>
@@ -3530,8 +4378,12 @@
       <c r="C214" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="215" spans="1:3">
+      <c r="F214">
+        <f>IF(AND(ISBLANK(D214), ISBLANK(E214)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6">
       <c r="A215" t="s">
         <v>205</v>
       </c>
@@ -3541,8 +4393,12 @@
       <c r="C215" s="2" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="216" spans="1:3">
+      <c r="F215">
+        <f>IF(AND(ISBLANK(D215), ISBLANK(E215)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6">
       <c r="A216" t="s">
         <v>205</v>
       </c>
@@ -3552,8 +4408,12 @@
       <c r="C216" s="2" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="217" spans="1:3">
+      <c r="F216">
+        <f>IF(AND(ISBLANK(D216), ISBLANK(E216)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6">
       <c r="A217" t="s">
         <v>205</v>
       </c>
@@ -3563,8 +4423,12 @@
       <c r="C217" s="2" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="218" spans="1:3">
+      <c r="F217">
+        <f>IF(AND(ISBLANK(D217), ISBLANK(E217)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6">
       <c r="A218" t="s">
         <v>205</v>
       </c>
@@ -3574,8 +4438,12 @@
       <c r="C218" s="2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="219" spans="1:3">
+      <c r="F218">
+        <f>IF(AND(ISBLANK(D218), ISBLANK(E218)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6">
       <c r="A219" t="s">
         <v>205</v>
       </c>
@@ -3585,8 +4453,12 @@
       <c r="C219" s="2" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="220" spans="1:3">
+      <c r="F219">
+        <f>IF(AND(ISBLANK(D219), ISBLANK(E219)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6">
       <c r="A220" t="s">
         <v>205</v>
       </c>
@@ -3596,8 +4468,12 @@
       <c r="C220" s="2" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="221" spans="1:3">
+      <c r="F220">
+        <f>IF(AND(ISBLANK(D220), ISBLANK(E220)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6">
       <c r="A221" t="s">
         <v>205</v>
       </c>
@@ -3607,8 +4483,12 @@
       <c r="C221" s="2" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="222" spans="1:3">
+      <c r="F221">
+        <f>IF(AND(ISBLANK(D221), ISBLANK(E221)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6">
       <c r="A222" t="s">
         <v>205</v>
       </c>
@@ -3618,8 +4498,12 @@
       <c r="C222" s="2" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="223" spans="1:3">
+      <c r="F222">
+        <f>IF(AND(ISBLANK(D222), ISBLANK(E222)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6">
       <c r="A223" t="s">
         <v>205</v>
       </c>
@@ -3629,8 +4513,12 @@
       <c r="C223" s="2" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="224" spans="1:3">
+      <c r="F223">
+        <f>IF(AND(ISBLANK(D223), ISBLANK(E223)), 1, "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6">
       <c r="A224" t="s">
         <v>205</v>
       </c>
@@ -3639,6 +4527,10 @@
       </c>
       <c r="C224" s="2" t="s">
         <v>251</v>
+      </c>
+      <c r="F224">
+        <f>IF(AND(ISBLANK(D224), ISBLANK(E224)), 1, "")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="225" spans="1:6">
@@ -3651,6 +4543,10 @@
       <c r="C225" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="F225">
+        <f>IF(AND(ISBLANK(D225), ISBLANK(E225)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="226" spans="1:6">
       <c r="A226" t="s">
@@ -3662,6 +4558,10 @@
       <c r="C226" s="2" t="s">
         <v>253</v>
       </c>
+      <c r="F226">
+        <f>IF(AND(ISBLANK(D226), ISBLANK(E226)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="227" spans="1:6">
       <c r="A227" t="s">
@@ -3673,6 +4573,10 @@
       <c r="C227" s="2" t="s">
         <v>254</v>
       </c>
+      <c r="F227">
+        <f>IF(AND(ISBLANK(D227), ISBLANK(E227)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="228" spans="1:6">
       <c r="A228" t="s">
@@ -3684,6 +4588,10 @@
       <c r="C228" s="2" t="s">
         <v>255</v>
       </c>
+      <c r="F228">
+        <f>IF(AND(ISBLANK(D228), ISBLANK(E228)), 1, "")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="229" spans="1:6">
       <c r="A229" t="s">
@@ -3694,6 +4602,10 @@
       </c>
       <c r="C229" s="2" t="s">
         <v>256</v>
+      </c>
+      <c r="F229">
+        <f>IF(AND(ISBLANK(D229), ISBLANK(E229)), 1, "")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="233" spans="1:6">

</xml_diff>